<commit_message>
update result, exp1, exp2, exp6
</commit_message>
<xml_diff>
--- a/Exp6/Result/TRADITIONAL method.xlsx
+++ b/Exp6/Result/TRADITIONAL method.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\zangyi\University\CUHK\2021summer\sustech\DeepSeparator\Exp6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\zangyi\University\CUHK\2021summer\sustech\DeepSeparator\Exp6\Result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220A4FBA-18C0-49D2-AAF2-274D4F22390D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45659FD-368C-4033-B74F-5C7D8148F6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{BFEFE3B0-4CAC-44DE-A52E-26BFDCA1F735}"/>
+    <workbookView xWindow="348" yWindow="348" windowWidth="2388" windowHeight="564" xr2:uid="{BFEFE3B0-4CAC-44DE-A52E-26BFDCA1F735}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="181" formatCode="0.0000000_);[Red]\(0.0000000\)"/>
+    <numFmt numFmtId="176" formatCode="0.0000000_);[Red]\(0.0000000\)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -137,13 +137,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -462,13 +462,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FF5FA3B-B5B5-4C71-81C6-4CA5B056DF50}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="44.109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="24.88671875" style="1" customWidth="1"/>
     <col min="3" max="3" width="25.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="21.44140625" style="1" customWidth="1"/>

</xml_diff>